<commit_message>
Final changes for draft manuscript
</commit_message>
<xml_diff>
--- a/docs/Key_for_post_processed_data_sheets.xlsx
+++ b/docs/Key_for_post_processed_data_sheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/derrick_muheki_vub_be/Documents/PhD_Derrick_Muheki/21_Research/21_6_Analysis/21_6_0_Preprocessing_data/Data_Rescue_Congo_DRC-1/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{223F88BB-2C26-4DFB-95A6-3277D609D1FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="8_{223F88BB-2C26-4DFB-95A6-3277D609D1FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88D48296-EAC2-46CF-B870-ECE6633123B0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21840" xr2:uid="{AEF280B1-861E-4CAE-9090-66589E223D19}"/>
+    <workbookView xWindow="-23148" yWindow="4188" windowWidth="23256" windowHeight="12456" xr2:uid="{AEF280B1-861E-4CAE-9090-66589E223D19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,30 +41,17 @@
     <t>Key</t>
   </si>
   <si>
-    <t>Description of original transcription</t>
+    <t>Values remain unchanged by the QA/QC checks, except for a special adjustment to ensure they match the required decimal places.</t>
   </si>
   <si>
-    <t>Unchanged in post processing.</t>
+    <t>The QA/QC checks confirmed that this transcription or correction is correct.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Had a word instead of a number. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Check this.</t>
-    </r>
+    <t>Description of original transcription and QA/QC flags</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Exceeds thresholds for maximum and minimum temperature. For temperatures in hundreds, the value was divided by 10 in the post processing. </t>
+      <t>Transcribed values for temperature, evaporation, or rainfall with more than three digits were adjusted to a maximum of three digits.</t>
     </r>
     <r>
       <rPr>
@@ -75,12 +62,111 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Check this.</t>
+      <t xml:space="preserve"> An expert transcriber is recommended to manually review this.</t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Total or average values are not equal to the sum or average of the transcribed daily values. </t>
+      <t xml:space="preserve">Transcribed temperature values did not meet the conditions: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>min</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &lt; </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ave</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &lt; </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>max</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
     </r>
     <r>
       <rPr>
@@ -91,15 +177,28 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Check this.</t>
+      <t xml:space="preserve"> An expert transcriber is recommended to manually review this.</t>
     </r>
   </si>
   <si>
-    <t>The total or average values confirmed that this transcription is correct.</t>
+    <r>
+      <t>Transcribed value exceeds thresholds for maximum and minimum temperature. For values in the hundreds, the value was divided by 10.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> An expert transcriber is recommended to manually review this.</t>
+    </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Had more than 1 decimal point. The first decimal point was eliminated in the post processing. </t>
+      <t xml:space="preserve">Transcribed total or average values do not match the sum or average of the transcribed daily values. </t>
     </r>
     <r>
       <rPr>
@@ -110,12 +209,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Check this</t>
+      <t>An expert transcriber is recommended to manually review this.</t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Transcribed data was manipulated by dividing by 10. </t>
+      <t xml:space="preserve">Total or average values were not transcribed or are missing. </t>
     </r>
     <r>
       <rPr>
@@ -126,7 +225,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Check this</t>
+      <t>An expert transcriber is recommended to manually review this.</t>
     </r>
   </si>
 </sst>
@@ -134,7 +233,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +249,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC0CB"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -157,12 +280,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -194,6 +311,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC0CB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -222,16 +345,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -240,6 +385,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFC0CB"/>
       <color rgb="FF6DCD57"/>
       <color rgb="FF75696F"/>
       <color rgb="FFCC3300"/>
@@ -249,7 +395,6 @@
       <color rgb="FFFFFFF0"/>
       <color rgb="FFF77509"/>
       <color rgb="FFFF0000"/>
-      <color rgb="FFFFFF00"/>
     </mruColors>
   </colors>
   <extLst>
@@ -263,8 +408,70 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>5814060</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D5416A0-BA73-1B78-5BCA-F268931DF7B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1203960" y="3489960"/>
+          <a:ext cx="6438900" cy="2644140"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -564,69 +771,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150A1D9E-732C-4A80-9638-BB4F720BB323}">
-  <dimension ref="C2:D9"/>
+  <dimension ref="C1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="137.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="84.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C2" s="8" t="s">
+    <row r="1" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="3:13" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="1"/>
+      <c r="D3" s="10" t="s">
         <v>1</v>
       </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
     </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
+    <row r="4" spans="3:13" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="4"/>
+      <c r="D4" s="10" t="s">
         <v>2</v>
       </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
     </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="6"/>
-      <c r="D4" s="1" t="s">
+    <row r="5" spans="3:13" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="5"/>
+      <c r="D5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="3:13" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="6"/>
+      <c r="D6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="3:13" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="7"/>
+      <c r="D7" s="10" t="s">
         <v>6</v>
       </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="2"/>
-      <c r="D5" s="1" t="s">
+    <row r="8" spans="3:13" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="8"/>
+      <c r="D8" s="10" t="s">
         <v>7</v>
       </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="3"/>
-      <c r="D6" s="1" t="s">
+    <row r="9" spans="3:13" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="9"/>
+      <c r="D9" s="10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="4"/>
-      <c r="D7" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="5"/>
-      <c r="D8" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="7"/>
-      <c r="D9" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>